<commit_message>
Initial version of BlancoTypeReference, NOT YET TESTED.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtClassGenericSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB08049-78FA-2B41-8682-8E50945DDB90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6442A66-DAC5-E648-A517-17C8D81E1CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6860" yWindow="1180" windowWidth="25440" windowHeight="18580" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="100">
   <si>
     <t>クラス名</t>
   </si>
@@ -561,6 +561,29 @@
   </si>
   <si>
     <t>blanco.sample.valueobjectkt.simple</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>仮想パラメータ</t>
+    <rPh sb="0" eb="2">
+      <t>カソウパラ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>※ このクラスで使用されている仮想パラメータ（カンマ区切り、TypeReference作成用）</t>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">シヨウサレテイル </t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t xml:space="preserve">カソウパラメータ </t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t xml:space="preserve">サクセイ </t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t xml:space="preserve">ヨウ </t>
+    </rPh>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1267,27 +1290,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1299,16 +1321,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1318,19 +1339,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1342,7 +1357,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1375,19 +1390,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1400,45 +1412,34 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1449,6 +1450,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1458,32 +1468,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1896,17 +1894,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S66"/>
+  <dimension ref="A1:S61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="6" width="23.5" style="1" customWidth="1"/>
-    <col min="7" max="9" width="20.1640625" style="28" customWidth="1"/>
+    <col min="7" max="9" width="20.1640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="23.5" style="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" style="1" customWidth="1"/>
     <col min="12" max="12" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -1937,10 +1935,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-    </row>
     <row r="5" spans="1:17">
       <c r="A5" s="3" t="s">
         <v>10</v>
@@ -1950,13 +1944,6 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="3" t="s">
@@ -1969,14 +1956,6 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="8"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="34"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="3" t="s">
@@ -1986,17 +1965,9 @@
       <c r="C7" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
       <c r="F7" s="11"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="34"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="3" t="s">
@@ -2006,17 +1977,9 @@
       <c r="C8" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
       <c r="F8" s="11"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="34"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="3" t="s">
@@ -2026,1216 +1989,1041 @@
       <c r="C9" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="33" t="s">
+      <c r="G9" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="34"/>
-    </row>
-    <row r="10" spans="1:17" ht="45">
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="45">
+      <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="68" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="11"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="34"/>
-    </row>
-    <row r="11" spans="1:17" ht="29" customHeight="1">
-      <c r="A11" s="3" t="s">
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:17" ht="29" customHeight="1">
+      <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="103" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="104"/>
-      <c r="E11" s="104"/>
-      <c r="F11" s="105"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="61"/>
-      <c r="N11" s="61"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="33"/>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="3" t="s">
+      <c r="D12" s="89"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="90"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="8"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="33"/>
-    </row>
-    <row r="13" spans="1:17" s="28" customFormat="1">
-      <c r="A13" s="58" t="s">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="60"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13" s="75"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="65"/>
-      <c r="O13"/>
-    </row>
-    <row r="14" spans="1:17" s="28" customFormat="1">
-      <c r="A14" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="60" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" t="s">
-        <v>62</v>
-      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="51"/>
+      <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="62"/>
-      <c r="K14" s="62"/>
-      <c r="L14" s="62"/>
-      <c r="M14" s="62"/>
-      <c r="N14" s="65"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
       <c r="O14"/>
     </row>
-    <row r="15" spans="1:17" s="28" customFormat="1">
-      <c r="A15" s="58" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="60"/>
-      <c r="D15"/>
+    <row r="15" spans="1:17">
+      <c r="A15" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
-      <c r="H15" s="75"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="62"/>
-      <c r="L15" s="62"/>
-      <c r="M15" s="62"/>
-      <c r="N15" s="65"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
       <c r="O15"/>
     </row>
-    <row r="16" spans="1:17" s="28" customFormat="1">
-      <c r="A16" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="59"/>
-      <c r="C16" s="60"/>
+    <row r="16" spans="1:17">
+      <c r="A16" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="51"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16"/>
-      <c r="H16" s="75"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="62"/>
-      <c r="M16" s="62"/>
-      <c r="N16" s="65"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
       <c r="O16"/>
     </row>
-    <row r="17" spans="1:19" s="28" customFormat="1">
-      <c r="A17" s="58" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="59"/>
-      <c r="C17" s="60" t="s">
-        <v>44</v>
-      </c>
+    <row r="17" spans="1:18">
+      <c r="A17" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="51"/>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="62"/>
-      <c r="L17" s="62"/>
-      <c r="M17" s="62"/>
-      <c r="N17" s="65"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
       <c r="O17"/>
     </row>
-    <row r="18" spans="1:19" s="28" customFormat="1">
-      <c r="A18" s="58" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="60" t="s">
+    <row r="18" spans="1:18">
+      <c r="A18" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="51" t="s">
         <v>44</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="62"/>
-      <c r="K18" s="62"/>
-      <c r="L18" s="62"/>
-      <c r="M18" s="62"/>
-      <c r="N18" s="65"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
       <c r="O18"/>
     </row>
-    <row r="19" spans="1:19" s="36" customFormat="1">
-      <c r="A19" s="33"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="76"/>
-      <c r="I19" s="76"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
-      <c r="Q19" s="33"/>
-    </row>
-    <row r="20" spans="1:19">
-      <c r="A20" s="26" t="s">
+    <row r="19" spans="1:18">
+      <c r="A19" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="B20"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="78"/>
-      <c r="G20" s="70"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="76"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="41"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="28"/>
-      <c r="R20" s="28"/>
-      <c r="S20" s="28"/>
-    </row>
-    <row r="21" spans="1:19">
-      <c r="A21" s="29" t="s">
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="31" t="s">
+      <c r="B22" s="28"/>
+      <c r="C22" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="79"/>
-      <c r="G21" s="70"/>
-      <c r="H21" s="76"/>
-      <c r="I21" s="76"/>
-      <c r="J21" s="63"/>
-      <c r="K21" s="63"/>
-      <c r="L21" s="63"/>
-      <c r="M21" s="63"/>
-      <c r="N21" s="63"/>
-      <c r="O21" s="63"/>
-      <c r="P21" s="28"/>
-      <c r="Q21" s="28"/>
-      <c r="R21" s="28"/>
-      <c r="S21" s="28"/>
-    </row>
-    <row r="22" spans="1:19">
-      <c r="A22" s="3" t="s">
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="53"/>
+      <c r="M22" s="53"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="53"/>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="10" t="s">
+      <c r="B23" s="6"/>
+      <c r="C23" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="80"/>
-      <c r="G22"/>
-      <c r="H22" s="75"/>
-      <c r="I22" s="75"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="34"/>
-    </row>
-    <row r="23" spans="1:19">
-      <c r="A23" s="3" t="s">
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="63"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="81"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="34"/>
-    </row>
-    <row r="24" spans="1:19">
-      <c r="A24" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="B24" s="6"/>
-      <c r="C24" s="7" t="s">
-        <v>73</v>
-      </c>
+      <c r="C24" s="7"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
-      <c r="F24" s="81"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="34"/>
-    </row>
-    <row r="25" spans="1:19">
-      <c r="A25" s="33"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="76"/>
-      <c r="I25" s="76"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
-      <c r="O25" s="34"/>
-    </row>
-    <row r="26" spans="1:19">
-      <c r="A26" s="26" t="s">
+      <c r="F24" s="64"/>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="64"/>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="B26"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="78"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="77"/>
-      <c r="I26" s="77"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="41"/>
-      <c r="P26" s="40"/>
-      <c r="Q26" s="40"/>
-      <c r="R26" s="40"/>
-      <c r="S26" s="40"/>
-    </row>
-    <row r="27" spans="1:19">
-      <c r="A27" s="44" t="s">
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="39" t="s">
+      <c r="B28" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="82"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="77"/>
-      <c r="I27" s="77"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="63"/>
-      <c r="L27" s="63"/>
-      <c r="M27" s="63"/>
-      <c r="N27" s="63"/>
-      <c r="O27" s="63"/>
-      <c r="P27" s="41"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="42"/>
-      <c r="S27" s="34"/>
-    </row>
-    <row r="28" spans="1:19">
-      <c r="A28" s="47"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="77"/>
-      <c r="I28" s="77"/>
-      <c r="J28" s="64"/>
-      <c r="K28" s="64"/>
-      <c r="L28" s="64"/>
-      <c r="M28" s="64"/>
-      <c r="N28" s="64"/>
-      <c r="O28" s="33"/>
-      <c r="P28" s="35"/>
-      <c r="Q28" s="35"/>
-      <c r="R28" s="35"/>
-      <c r="S28" s="34"/>
-    </row>
-    <row r="29" spans="1:19">
-      <c r="A29" s="47"/>
-      <c r="B29" s="43"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="84"/>
-      <c r="G29"/>
-      <c r="H29" s="75"/>
-      <c r="I29" s="75"/>
-      <c r="J29" s="64"/>
-      <c r="K29" s="64"/>
-      <c r="L29" s="64"/>
-      <c r="M29" s="64"/>
-      <c r="N29" s="64"/>
-      <c r="O29" s="33"/>
-      <c r="P29" s="35"/>
-      <c r="Q29" s="35"/>
-      <c r="R29" s="35"/>
-      <c r="S29" s="34"/>
-    </row>
-    <row r="30" spans="1:19">
-      <c r="A30" s="48"/>
-      <c r="B30" s="45"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="85"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="64"/>
-      <c r="K30" s="64"/>
-      <c r="L30" s="64"/>
-      <c r="M30" s="64"/>
-      <c r="N30" s="64"/>
-      <c r="O30" s="33"/>
-      <c r="P30" s="35"/>
-      <c r="Q30" s="35"/>
-      <c r="R30" s="35"/>
-      <c r="S30" s="34"/>
-    </row>
-    <row r="31" spans="1:19" s="36" customFormat="1">
-      <c r="A31" s="33"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="33"/>
-      <c r="N31" s="33"/>
-      <c r="O31" s="33"/>
-      <c r="P31" s="33"/>
-      <c r="Q31" s="33"/>
-    </row>
-    <row r="32" spans="1:19" s="28" customFormat="1">
-      <c r="A32" s="96" t="s">
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="53"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="53"/>
+      <c r="O28" s="53"/>
+      <c r="Q28" s="34"/>
+      <c r="R28" s="34"/>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="39"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="54"/>
+      <c r="M29" s="54"/>
+      <c r="N29" s="54"/>
+      <c r="P29"/>
+      <c r="Q29"/>
+      <c r="R29"/>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" s="39"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="67"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30" s="54"/>
+      <c r="K30" s="54"/>
+      <c r="L30" s="54"/>
+      <c r="M30" s="54"/>
+      <c r="N30" s="54"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+      <c r="R30"/>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="40"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="68"/>
+      <c r="J31" s="54"/>
+      <c r="K31" s="54"/>
+      <c r="L31" s="54"/>
+      <c r="M31" s="54"/>
+      <c r="N31" s="54"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="B32"/>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B32" s="59"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="97"/>
-    </row>
-    <row r="33" spans="1:19" s="28" customFormat="1">
-      <c r="A33" s="107" t="s">
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="79"/>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" s="86" t="s">
         <v>87</v>
       </c>
-      <c r="B33" s="107" t="s">
+      <c r="B34" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="113" t="s">
+      <c r="C34" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="113" t="s">
+      <c r="D34" s="87" t="s">
         <v>88</v>
       </c>
-      <c r="E33" s="113" t="s">
+      <c r="E34" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="F33" s="114"/>
-      <c r="G33" s="70"/>
-      <c r="H33" s="70"/>
-      <c r="I33" s="70"/>
-      <c r="J33" s="70"/>
-      <c r="K33" s="70"/>
-    </row>
-    <row r="34" spans="1:19" s="28" customFormat="1">
-      <c r="A34" s="107"/>
-      <c r="B34" s="107"/>
-      <c r="C34" s="113"/>
-      <c r="D34" s="113"/>
-      <c r="E34" s="113"/>
-      <c r="F34" s="114"/>
-      <c r="G34" s="70"/>
-      <c r="H34" s="70"/>
-      <c r="I34" s="70"/>
-      <c r="J34" s="70"/>
-      <c r="K34" s="70"/>
-    </row>
-    <row r="35" spans="1:19" s="28" customFormat="1">
-      <c r="A35" s="19">
+      <c r="F34" s="85"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="53"/>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="A35" s="86"/>
+      <c r="B35" s="86"/>
+      <c r="C35" s="87"/>
+      <c r="D35" s="87"/>
+      <c r="E35" s="87"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="53"/>
+      <c r="K35" s="53"/>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="A36" s="18">
         <v>1</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B36" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="73" t="s">
+      <c r="C36" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="D35" s="73" t="s">
+      <c r="D36" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E35" s="73" t="s">
+      <c r="E36" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="F35" s="101"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="70"/>
-      <c r="I35" s="70"/>
-      <c r="J35" s="70"/>
-      <c r="K35" s="70"/>
-      <c r="L35" s="70"/>
-    </row>
-    <row r="36" spans="1:19" s="28" customFormat="1">
-      <c r="A36" s="19"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="73"/>
-      <c r="D36" s="73"/>
-      <c r="E36" s="73"/>
-      <c r="F36" s="101"/>
-      <c r="G36" s="70"/>
-      <c r="H36" s="70"/>
-      <c r="I36" s="70"/>
-      <c r="J36" s="70"/>
-      <c r="K36" s="70"/>
-      <c r="L36" s="70"/>
-    </row>
-    <row r="37" spans="1:19" s="28" customFormat="1">
-      <c r="A37" s="19"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="73"/>
-      <c r="D37" s="73"/>
-      <c r="E37" s="73"/>
-      <c r="F37" s="101"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="70"/>
-      <c r="I37" s="70"/>
-      <c r="J37" s="70"/>
-      <c r="K37" s="70"/>
-      <c r="L37" s="70"/>
-    </row>
-    <row r="38" spans="1:19" s="28" customFormat="1">
-      <c r="A38" s="19"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="73"/>
-      <c r="D38" s="73"/>
-      <c r="E38" s="73"/>
-      <c r="F38" s="101"/>
-      <c r="G38" s="70"/>
-      <c r="H38" s="70"/>
-      <c r="I38" s="70"/>
-      <c r="J38" s="70"/>
-      <c r="K38" s="70"/>
-      <c r="L38" s="70"/>
-    </row>
-    <row r="39" spans="1:19" s="28" customFormat="1">
-      <c r="A39" s="19"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="73"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="101"/>
-      <c r="G39" s="70"/>
-      <c r="H39" s="70"/>
-      <c r="I39" s="70"/>
-      <c r="J39" s="70"/>
-      <c r="K39" s="70"/>
-      <c r="L39" s="70"/>
-    </row>
-    <row r="40" spans="1:19" s="28" customFormat="1">
-      <c r="A40" s="98"/>
-      <c r="B40" s="99"/>
-      <c r="C40" s="100"/>
-      <c r="D40" s="100"/>
-      <c r="E40" s="100"/>
-      <c r="F40" s="102"/>
-      <c r="G40" s="70"/>
-      <c r="H40" s="70"/>
-      <c r="I40" s="70"/>
-      <c r="J40" s="70"/>
-      <c r="K40" s="70"/>
-      <c r="L40" s="70"/>
-    </row>
-    <row r="41" spans="1:19" s="28" customFormat="1">
-      <c r="A41"/>
-      <c r="B41"/>
-      <c r="C41"/>
-      <c r="D41"/>
-      <c r="E41"/>
-      <c r="F41"/>
-      <c r="G41"/>
-      <c r="H41"/>
-      <c r="I41"/>
-      <c r="J41"/>
-      <c r="K41"/>
-      <c r="L41" s="71"/>
-      <c r="M41"/>
-    </row>
-    <row r="42" spans="1:19">
-      <c r="A42" s="26" t="s">
+      <c r="F36" s="83"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="53"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="53"/>
+      <c r="L36" s="53"/>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="A37" s="18"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="83"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="53"/>
+      <c r="L37" s="53"/>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38" s="18"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="83"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="53"/>
+      <c r="J38" s="53"/>
+      <c r="K38" s="53"/>
+      <c r="L38" s="53"/>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39" s="18"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="83"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="53"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="53"/>
+      <c r="L39" s="53"/>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40" s="18"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="83"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="53"/>
+      <c r="K40" s="53"/>
+      <c r="L40" s="53"/>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41" s="80"/>
+      <c r="B41" s="81"/>
+      <c r="C41" s="82"/>
+      <c r="D41" s="82"/>
+      <c r="E41" s="82"/>
+      <c r="F41" s="84"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="53"/>
+      <c r="J41" s="53"/>
+      <c r="K41" s="53"/>
+      <c r="L41" s="53"/>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="A42"/>
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42" s="54"/>
+      <c r="M42"/>
+    </row>
+    <row r="43" spans="1:18">
+      <c r="A43" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="78"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="40"/>
-      <c r="J42" s="41"/>
-      <c r="K42" s="41"/>
-      <c r="L42" s="41"/>
-      <c r="M42" s="41"/>
-      <c r="N42" s="41"/>
-      <c r="O42" s="41"/>
-      <c r="P42" s="40"/>
-      <c r="Q42" s="40"/>
-      <c r="R42" s="40"/>
-      <c r="S42" s="40"/>
-    </row>
-    <row r="43" spans="1:19">
-      <c r="A43" s="44" t="s">
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="61"/>
+    </row>
+    <row r="44" spans="1:18">
+      <c r="A44" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="39" t="s">
+      <c r="B44" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="82"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="63"/>
-      <c r="K43" s="63"/>
-      <c r="L43" s="63"/>
-      <c r="M43" s="63"/>
-      <c r="N43" s="63"/>
-      <c r="O43" s="63"/>
-      <c r="P43" s="41"/>
-      <c r="Q43" s="42"/>
-      <c r="R43" s="42"/>
-      <c r="S43" s="34"/>
-    </row>
-    <row r="44" spans="1:19">
-      <c r="A44" s="47">
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="65"/>
+      <c r="J44" s="53"/>
+      <c r="K44" s="53"/>
+      <c r="L44" s="53"/>
+      <c r="M44" s="53"/>
+      <c r="N44" s="53"/>
+      <c r="O44" s="53"/>
+      <c r="Q44" s="34"/>
+      <c r="R44" s="34"/>
+    </row>
+    <row r="45" spans="1:18">
+      <c r="A45" s="39">
         <v>1</v>
       </c>
-      <c r="B44" s="43" t="s">
+      <c r="B45" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="83"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="64"/>
-      <c r="K44" s="64"/>
-      <c r="L44" s="64"/>
-      <c r="M44" s="64"/>
-      <c r="N44" s="64"/>
-      <c r="O44" s="33"/>
-      <c r="P44" s="35"/>
-      <c r="Q44" s="35"/>
-      <c r="R44" s="35"/>
-      <c r="S44" s="34"/>
-    </row>
-    <row r="45" spans="1:19">
-      <c r="A45" s="47"/>
-      <c r="B45" s="43"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="84"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="64"/>
-      <c r="K45" s="64"/>
-      <c r="L45" s="64"/>
-      <c r="M45" s="64"/>
-      <c r="N45" s="64"/>
-      <c r="O45" s="33"/>
-      <c r="P45" s="35"/>
-      <c r="Q45" s="35"/>
-      <c r="R45" s="35"/>
-      <c r="S45" s="34"/>
-    </row>
-    <row r="46" spans="1:19">
-      <c r="A46" s="48"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="85"/>
-      <c r="H46" s="40"/>
-      <c r="I46" s="40"/>
-      <c r="J46" s="64"/>
-      <c r="K46" s="64"/>
-      <c r="L46" s="64"/>
-      <c r="M46" s="64"/>
-      <c r="N46" s="64"/>
-      <c r="O46" s="33"/>
-      <c r="P46" s="35"/>
-      <c r="Q46" s="35"/>
-      <c r="R46" s="35"/>
-      <c r="S46" s="34"/>
-    </row>
-    <row r="47" spans="1:19">
-      <c r="A47" s="13"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="J47" s="13"/>
-      <c r="K47" s="13"/>
-      <c r="L47" s="13"/>
-      <c r="M47" s="13"/>
-      <c r="N47" s="13"/>
-      <c r="O47" s="13"/>
-      <c r="P47" s="13"/>
-    </row>
-    <row r="48" spans="1:19">
-      <c r="A48" s="3" t="s">
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="66"/>
+      <c r="J45" s="54"/>
+      <c r="K45" s="54"/>
+      <c r="L45" s="54"/>
+      <c r="M45" s="54"/>
+      <c r="N45" s="54"/>
+      <c r="P45"/>
+      <c r="Q45"/>
+      <c r="R45"/>
+    </row>
+    <row r="46" spans="1:18">
+      <c r="A46" s="39"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="67"/>
+      <c r="J46" s="54"/>
+      <c r="K46" s="54"/>
+      <c r="L46" s="54"/>
+      <c r="M46" s="54"/>
+      <c r="N46" s="54"/>
+      <c r="P46"/>
+      <c r="Q46"/>
+      <c r="R46"/>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47" s="40"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="68"/>
+      <c r="J47" s="54"/>
+      <c r="K47" s="54"/>
+      <c r="L47" s="54"/>
+      <c r="M47" s="54"/>
+      <c r="N47" s="54"/>
+      <c r="P47"/>
+      <c r="Q47"/>
+      <c r="R47"/>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="A48"/>
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
+      <c r="O48"/>
+      <c r="P48"/>
+    </row>
+    <row r="49" spans="1:19">
+      <c r="A49" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="59"/>
-      <c r="H48" s="59"/>
-      <c r="I48" s="59"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
-      <c r="P48" s="14"/>
-      <c r="Q48" s="14"/>
-      <c r="R48" s="6"/>
-      <c r="S48" s="15"/>
-    </row>
-    <row r="49" spans="1:19" ht="13.5" customHeight="1">
-      <c r="A49" s="107" t="s">
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="13"/>
+      <c r="P49" s="13"/>
+      <c r="Q49" s="13"/>
+      <c r="R49" s="6"/>
+      <c r="S49" s="14"/>
+    </row>
+    <row r="50" spans="1:19" ht="13.5" customHeight="1">
+      <c r="A50" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="B49" s="107" t="s">
+      <c r="B50" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="C49" s="106" t="s">
+      <c r="C50" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="106" t="s">
+      <c r="D50" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="E49" s="108" t="s">
+      <c r="E50" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="F49" s="106" t="s">
+      <c r="F50" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="G49" s="113" t="s">
+      <c r="G50" s="87" t="s">
         <v>81</v>
       </c>
-      <c r="H49" s="113" t="s">
+      <c r="H50" s="87" t="s">
         <v>82</v>
       </c>
-      <c r="I49" s="113" t="s">
+      <c r="I50" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="J49" s="106" t="s">
+      <c r="J50" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="K49" s="108" t="s">
+      <c r="K50" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="L49" s="108" t="s">
+      <c r="L50" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="M49" s="111" t="s">
+      <c r="M50" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="N49" s="111" t="s">
+      <c r="N50" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="O49" s="106" t="s">
+      <c r="O50" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="P49" s="106"/>
-      <c r="Q49" s="16"/>
-      <c r="R49" s="17"/>
-      <c r="S49" s="9"/>
-    </row>
-    <row r="50" spans="1:19">
-      <c r="A50" s="107"/>
-      <c r="B50" s="107"/>
-      <c r="C50" s="106"/>
-      <c r="D50" s="106"/>
-      <c r="E50" s="109"/>
-      <c r="F50" s="106"/>
-      <c r="G50" s="113"/>
-      <c r="H50" s="113"/>
-      <c r="I50" s="113"/>
-      <c r="J50" s="106"/>
-      <c r="K50" s="110"/>
-      <c r="L50" s="110"/>
-      <c r="M50" s="112"/>
-      <c r="N50" s="112"/>
-      <c r="O50" s="106"/>
-      <c r="P50" s="106"/>
-      <c r="Q50" s="18"/>
-      <c r="R50" s="25"/>
-      <c r="S50" s="15"/>
+      <c r="P50" s="87"/>
+      <c r="Q50" s="15"/>
+      <c r="R50" s="16"/>
+      <c r="S50" s="9"/>
     </row>
     <row r="51" spans="1:19">
-      <c r="A51" s="19">
+      <c r="A51" s="86"/>
+      <c r="B51" s="86"/>
+      <c r="C51" s="87"/>
+      <c r="D51" s="87"/>
+      <c r="E51" s="92"/>
+      <c r="F51" s="87"/>
+      <c r="G51" s="87"/>
+      <c r="H51" s="87"/>
+      <c r="I51" s="87"/>
+      <c r="J51" s="87"/>
+      <c r="K51" s="93"/>
+      <c r="L51" s="93"/>
+      <c r="M51" s="95"/>
+      <c r="N51" s="95"/>
+      <c r="O51" s="87"/>
+      <c r="P51" s="87"/>
+      <c r="Q51" s="17"/>
+      <c r="R51" s="24"/>
+      <c r="S51" s="14"/>
+    </row>
+    <row r="52" spans="1:19">
+      <c r="A52" s="18">
         <v>1</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B52" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="21" t="s">
+      <c r="C52" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21" t="s">
+      <c r="D52" s="20"/>
+      <c r="E52" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F51" s="21" t="s">
+      <c r="F52" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G51" s="72"/>
-      <c r="H51" s="72"/>
-      <c r="I51" s="72"/>
-      <c r="J51" s="21" t="s">
+      <c r="G52" s="59"/>
+      <c r="H52" s="59"/>
+      <c r="I52" s="59"/>
+      <c r="J52" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="K51" s="21"/>
-      <c r="L51" s="66"/>
-      <c r="M51" s="66" t="s">
+      <c r="K52" s="20"/>
+      <c r="L52" s="55"/>
+      <c r="M52" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="N51" s="66" t="s">
+      <c r="N52" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="O51" s="21" t="s">
+      <c r="O52" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="P51" s="22"/>
-      <c r="Q51" s="22"/>
-      <c r="R51" s="24"/>
-      <c r="S51" s="15"/>
-    </row>
-    <row r="52" spans="1:19" ht="60">
-      <c r="A52" s="19">
-        <f>A51+1</f>
+      <c r="P52" s="21"/>
+      <c r="Q52" s="21"/>
+      <c r="R52" s="23"/>
+      <c r="S52" s="14"/>
+    </row>
+    <row r="53" spans="1:19" ht="60">
+      <c r="A53" s="18">
+        <f>A52+1</f>
         <v>2</v>
       </c>
-      <c r="B52" s="20" t="s">
+      <c r="B53" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="21" t="s">
+      <c r="C53" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="21"/>
-      <c r="E52" s="69" t="s">
+      <c r="D53" s="20"/>
+      <c r="E53" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="F52" s="21"/>
-      <c r="G52" s="73"/>
-      <c r="H52" s="73"/>
-      <c r="I52" s="73"/>
-      <c r="J52" s="21">
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="20">
         <v>0</v>
       </c>
-      <c r="K52" s="21"/>
-      <c r="L52" s="66"/>
-      <c r="M52" s="66"/>
-      <c r="N52" s="66" t="s">
+      <c r="K53" s="20"/>
+      <c r="L53" s="55"/>
+      <c r="M53" s="55"/>
+      <c r="N53" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="O52" s="21"/>
-      <c r="P52" s="22"/>
-      <c r="Q52" s="22"/>
-      <c r="R52" s="24"/>
-      <c r="S52" s="15"/>
-    </row>
-    <row r="53" spans="1:19">
-      <c r="A53" s="19">
-        <f t="shared" ref="A53:A57" si="0">A52+1</f>
+      <c r="O53" s="20"/>
+      <c r="P53" s="21"/>
+      <c r="Q53" s="21"/>
+      <c r="R53" s="23"/>
+      <c r="S53" s="14"/>
+    </row>
+    <row r="54" spans="1:19">
+      <c r="A54" s="18">
+        <f t="shared" ref="A54:A58" si="0">A53+1</f>
         <v>3</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B54" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C53" s="21" t="s">
+      <c r="C54" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D53" s="21" t="s">
+      <c r="D54" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21" t="s">
+      <c r="E54" s="20"/>
+      <c r="F54" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="G53" s="73"/>
-      <c r="H53" s="73"/>
-      <c r="I53" s="73"/>
-      <c r="J53" s="21" t="s">
+      <c r="G54" s="20"/>
+      <c r="H54" s="20"/>
+      <c r="I54" s="20"/>
+      <c r="J54" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="K53" s="21"/>
-      <c r="L53" s="66" t="s">
+      <c r="K54" s="20"/>
+      <c r="L54" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="M53" s="66"/>
-      <c r="N53" s="66"/>
-      <c r="O53" s="21" t="s">
+      <c r="M54" s="55"/>
+      <c r="N54" s="55"/>
+      <c r="O54" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="P53" s="22"/>
-      <c r="Q53" s="22"/>
-      <c r="R53" s="23"/>
-      <c r="S53" s="15"/>
-    </row>
-    <row r="54" spans="1:19" ht="30">
-      <c r="A54" s="19">
+      <c r="P54" s="21"/>
+      <c r="Q54" s="21"/>
+      <c r="R54" s="22"/>
+      <c r="S54" s="14"/>
+    </row>
+    <row r="55" spans="1:19" ht="30">
+      <c r="A55" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B55" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C54" s="21" t="s">
+      <c r="C55" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D54" s="21"/>
-      <c r="E54" s="69" t="s">
+      <c r="D55" s="20"/>
+      <c r="E55" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="F54" s="21" t="s">
+      <c r="F55" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="G54" s="73"/>
-      <c r="H54" s="73"/>
-      <c r="I54" s="73"/>
-      <c r="J54" s="21"/>
-      <c r="K54" s="21"/>
-      <c r="L54" s="66"/>
-      <c r="M54" s="66"/>
-      <c r="N54" s="66"/>
-      <c r="O54" s="21" t="s">
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="20"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="55"/>
+      <c r="M55" s="55"/>
+      <c r="N55" s="55"/>
+      <c r="O55" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="P54" s="22"/>
-      <c r="Q54" s="22"/>
-      <c r="R54" s="23"/>
-      <c r="S54" s="15"/>
-    </row>
-    <row r="55" spans="1:19" ht="15">
-      <c r="A55" s="19">
+      <c r="P55" s="21"/>
+      <c r="Q55" s="21"/>
+      <c r="R55" s="22"/>
+      <c r="S55" s="14"/>
+    </row>
+    <row r="56" spans="1:19" ht="15">
+      <c r="A56" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B55" s="20" t="s">
+      <c r="B56" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C55" s="21" t="s">
+      <c r="C56" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D55" s="21"/>
-      <c r="E55" s="67" t="s">
+      <c r="D56" s="20"/>
+      <c r="E56" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="F55" s="21"/>
-      <c r="G55" s="74"/>
-      <c r="H55" s="74"/>
-      <c r="I55" s="74"/>
-      <c r="J55" s="21" t="s">
+      <c r="F56" s="20"/>
+      <c r="G56" s="60"/>
+      <c r="H56" s="60"/>
+      <c r="I56" s="60"/>
+      <c r="J56" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="K55" s="21"/>
-      <c r="L55" s="66"/>
-      <c r="M55" s="66"/>
-      <c r="N55" s="66"/>
-      <c r="O55" s="21" t="s">
+      <c r="K56" s="20"/>
+      <c r="L56" s="55"/>
+      <c r="M56" s="55"/>
+      <c r="N56" s="55"/>
+      <c r="O56" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="P55" s="22"/>
-      <c r="Q55" s="22"/>
-      <c r="R55" s="23"/>
-      <c r="S55" s="15"/>
-    </row>
-    <row r="56" spans="1:19" ht="30">
-      <c r="A56" s="19">
+      <c r="P56" s="21"/>
+      <c r="Q56" s="21"/>
+      <c r="R56" s="22"/>
+      <c r="S56" s="14"/>
+    </row>
+    <row r="57" spans="1:19" ht="30">
+      <c r="A57" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B56" s="92" t="s">
+      <c r="B57" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="C56" s="21" t="s">
+      <c r="C57" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="D56" s="21" t="s">
+      <c r="D57" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21" t="s">
+      <c r="E57" s="20"/>
+      <c r="F57" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="G56" s="73" t="s">
+      <c r="G57" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="H56" s="73"/>
-      <c r="I56" s="69" t="s">
+      <c r="H57" s="20"/>
+      <c r="I57" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="J56" s="21"/>
-      <c r="K56" s="21"/>
-      <c r="L56" s="66" t="s">
+      <c r="J57" s="20"/>
+      <c r="K57" s="20"/>
+      <c r="L57" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="M56" s="66"/>
-      <c r="N56" s="66" t="s">
+      <c r="M57" s="55"/>
+      <c r="N57" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="O56" s="21" t="s">
+      <c r="O57" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="P56" s="22"/>
-      <c r="Q56" s="22"/>
-      <c r="R56" s="23"/>
-      <c r="S56" s="15"/>
-    </row>
-    <row r="57" spans="1:19">
-      <c r="A57" s="19">
+      <c r="P57" s="21"/>
+      <c r="Q57" s="21"/>
+      <c r="R57" s="22"/>
+      <c r="S57" s="14"/>
+    </row>
+    <row r="58" spans="1:19">
+      <c r="A58" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B57" s="92" t="s">
+      <c r="B58" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="C57" s="21" t="s">
+      <c r="C58" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D57" s="21" t="s">
+      <c r="D58" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="73"/>
-      <c r="H57" s="73"/>
-      <c r="I57" s="69"/>
-      <c r="J57" s="21"/>
-      <c r="K57" s="21"/>
-      <c r="L57" s="66" t="s">
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="58"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="20"/>
+      <c r="L58" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="M57" s="66"/>
-      <c r="N57" s="66" t="s">
+      <c r="M58" s="55"/>
+      <c r="N58" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="O57" s="21" t="s">
+      <c r="O58" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="P57" s="22"/>
-      <c r="Q57" s="22"/>
-      <c r="R57" s="23"/>
-      <c r="S57" s="15"/>
-    </row>
-    <row r="58" spans="1:19">
-      <c r="A58" s="86"/>
-      <c r="B58" s="87"/>
-      <c r="C58" s="88"/>
-      <c r="D58" s="88"/>
-      <c r="E58" s="88"/>
-      <c r="F58" s="88"/>
-      <c r="G58" s="94"/>
-      <c r="H58" s="95"/>
-      <c r="I58" s="95"/>
-      <c r="J58" s="88"/>
-      <c r="K58" s="88"/>
-      <c r="L58" s="89"/>
-      <c r="M58" s="89"/>
-      <c r="N58" s="89"/>
-      <c r="O58" s="88"/>
-      <c r="P58" s="90"/>
-      <c r="Q58" s="90"/>
-      <c r="R58" s="91"/>
-      <c r="S58" s="15"/>
+      <c r="P58" s="21"/>
+      <c r="Q58" s="21"/>
+      <c r="R58" s="22"/>
+      <c r="S58" s="14"/>
     </row>
     <row r="59" spans="1:19">
-      <c r="G59" s="41"/>
-      <c r="H59" s="41"/>
-      <c r="I59" s="41"/>
-    </row>
-    <row r="60" spans="1:19">
-      <c r="G60" s="93"/>
-      <c r="H60" s="93"/>
-      <c r="I60" s="93"/>
+      <c r="A59" s="69"/>
+      <c r="B59" s="70"/>
+      <c r="C59" s="71"/>
+      <c r="D59" s="71"/>
+      <c r="E59" s="71"/>
+      <c r="F59" s="71"/>
+      <c r="G59" s="77"/>
+      <c r="H59" s="78"/>
+      <c r="I59" s="78"/>
+      <c r="J59" s="71"/>
+      <c r="K59" s="71"/>
+      <c r="L59" s="72"/>
+      <c r="M59" s="72"/>
+      <c r="N59" s="72"/>
+      <c r="O59" s="71"/>
+      <c r="P59" s="73"/>
+      <c r="Q59" s="73"/>
+      <c r="R59" s="74"/>
+      <c r="S59" s="14"/>
     </row>
     <row r="61" spans="1:19">
-      <c r="G61" s="41"/>
-      <c r="H61" s="41"/>
-      <c r="I61" s="41"/>
-    </row>
-    <row r="62" spans="1:19">
-      <c r="G62" s="41"/>
-      <c r="H62" s="41"/>
-      <c r="I62" s="41"/>
-    </row>
-    <row r="63" spans="1:19">
-      <c r="G63" s="41"/>
-      <c r="H63" s="41"/>
-      <c r="I63" s="41"/>
-    </row>
-    <row r="64" spans="1:19">
-      <c r="G64" s="41"/>
-      <c r="H64" s="41"/>
-      <c r="I64" s="41"/>
-    </row>
-    <row r="65" spans="7:9">
-      <c r="G65" s="41"/>
-      <c r="H65" s="41"/>
-      <c r="I65" s="41"/>
-    </row>
-    <row r="66" spans="7:9">
-      <c r="G66" s="41"/>
-      <c r="H66" s="41"/>
-      <c r="I66" s="41"/>
+      <c r="G61" s="76"/>
+      <c r="H61" s="76"/>
+      <c r="I61" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="O49:P50"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="L49:L50"/>
-    <mergeCell ref="N49:N50"/>
-    <mergeCell ref="M49:M50"/>
-    <mergeCell ref="K49:K50"/>
-    <mergeCell ref="J49:J50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="I49:I50"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="O50:P51"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="L50:L51"/>
+    <mergeCell ref="N50:N51"/>
+    <mergeCell ref="M50:M51"/>
+    <mergeCell ref="K50:K51"/>
+    <mergeCell ref="J50:J51"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="I50:I51"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F74 J74:N74" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F75 J75:N75" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17" xr:uid="{643F6C9A-8760-224C-A7F5-6893BC2E6C68}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18" xr:uid="{643F6C9A-8760-224C-A7F5-6893BC2E6C68}">
       <formula1>createToString</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15 K51:K58" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16 K52:K59" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>isAbstract</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{061A2328-C320-074B-A7A0-1D5ADA23E625}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17" xr:uid="{061A2328-C320-074B-A7A0-1D5ADA23E625}">
       <formula1>isFinal</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{2D8A5CB0-577F-DA47-9664-36C261082ADA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{2D8A5CB0-577F-DA47-9664-36C261082ADA}">
       <formula1>isData</formula1>
     </dataValidation>
   </dataValidations>
@@ -3251,7 +3039,7 @@
           <x14:formula1>
             <xm:f>config!$P$4:$P$5</xm:f>
           </x14:formula1>
-          <xm:sqref>L51:N58</xm:sqref>
+          <xm:sqref>L52:N59</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3272,107 +3060,107 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="51" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="51" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="51" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="51" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" style="51" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="51" customWidth="1"/>
-    <col min="10" max="10" width="18.5" style="51" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="51" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="51" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="15" max="260" width="8.83203125" style="51" customWidth="1"/>
-    <col min="261" max="16384" width="10.83203125" style="51"/>
+    <col min="1" max="3" width="8.83203125" style="43" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="43" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="43" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="43" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" style="43" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="43" customWidth="1"/>
+    <col min="10" max="10" width="18.5" style="43" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="43" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="43" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="15" max="260" width="8.83203125" style="43" customWidth="1"/>
+    <col min="261" max="16384" width="10.83203125" style="43"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="50" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="50"/>
+      <c r="Q1" s="42"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="52" t="s">
+      <c r="J3" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="52" t="s">
+      <c r="L3" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="52" t="s">
+      <c r="N3" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="P3" s="52" t="s">
+      <c r="P3" s="44" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="B4" s="53"/>
-      <c r="D4" s="56" t="s">
+      <c r="B4" s="45"/>
+      <c r="D4" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="N4" s="54"/>
-      <c r="P4" s="54"/>
+      <c r="H4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="P4" s="46"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="H5" s="56" t="s">
+      <c r="D5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="H5" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="56" t="s">
+      <c r="J5" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="L5" s="56" t="s">
+      <c r="L5" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="N5" s="56" t="s">
+      <c r="N5" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="P5" s="56" t="s">
+      <c r="P5" s="48" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="B6" s="57"/>
+      <c r="B6" s="49"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>

</xml_diff>